<commit_message>
Script4 running succesful-final changes
</commit_message>
<xml_diff>
--- a/Resources/4-data.xlsx
+++ b/Resources/4-data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="4605" windowWidth="20580" windowHeight="4665"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
   <si>
     <t>WH_NUMBER</t>
   </si>
@@ -392,7 +392,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,8 +528,8 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
+      <c r="B12" s="2">
+        <v>1205356</v>
       </c>
       <c r="C12" s="1">
         <v>2716812</v>

</xml_diff>

<commit_message>
script4-added image if needed
</commit_message>
<xml_diff>
--- a/Resources/4-data.xlsx
+++ b/Resources/4-data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="5280"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20580" windowHeight="5280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,43 +45,43 @@
     <t>1213989</t>
   </si>
   <si>
+    <t>1774139</t>
+  </si>
+  <si>
+    <t>1774140</t>
+  </si>
+  <si>
+    <t>1774141</t>
+  </si>
+  <si>
+    <t>1774123</t>
+  </si>
+  <si>
+    <t>1774124</t>
+  </si>
+  <si>
+    <t>1774125</t>
+  </si>
+  <si>
+    <t>1774126</t>
+  </si>
+  <si>
+    <t>1774127</t>
+  </si>
+  <si>
+    <t>1774128</t>
+  </si>
+  <si>
+    <t>1774129</t>
+  </si>
+  <si>
+    <t>1774130</t>
+  </si>
+  <si>
+    <t>1774131</t>
+  </si>
+  <si>
     <t>1774138</t>
-  </si>
-  <si>
-    <t>1774139</t>
-  </si>
-  <si>
-    <t>1774140</t>
-  </si>
-  <si>
-    <t>1774141</t>
-  </si>
-  <si>
-    <t>1774123</t>
-  </si>
-  <si>
-    <t>1774124</t>
-  </si>
-  <si>
-    <t>1774125</t>
-  </si>
-  <si>
-    <t>1774126</t>
-  </si>
-  <si>
-    <t>1774127</t>
-  </si>
-  <si>
-    <t>1774128</t>
-  </si>
-  <si>
-    <t>1774129</t>
-  </si>
-  <si>
-    <t>1774130</t>
-  </si>
-  <si>
-    <t>1774131</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -543,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -554,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -565,7 +565,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -576,7 +576,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -587,7 +587,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -598,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -642,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -653,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -666,9 +666,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>